<commit_message>
Add ETL process for cleaning movie data.  columns are mapped/merged and budget is clean.
</commit_message>
<xml_diff>
--- a/analysis/wiki column mapping.xlsx
+++ b/analysis/wiki column mapping.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git repos\movies_ETL\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27069685-D0F5-4B12-B977-24D1730ADDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{461C06A6-94A2-4CF1-8161-AE951837CC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D61B07E9-75AC-4A64-AB41-EFCCFD051A2F}"/>
+    <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11235" xr2:uid="{D61B07E9-75AC-4A64-AB41-EFCCFD051A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -588,10 +589,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4460966F-A681-4CC4-9BC5-D71793F5778B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A13" sqref="A13:B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -612,7 +614,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" hidden="1">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -621,7 +623,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" hidden="1">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -630,7 +632,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" hidden="1">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -639,7 +641,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" hidden="1">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -648,7 +650,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" hidden="1">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -657,7 +659,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" hidden="1">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -666,7 +668,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" hidden="1">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -675,7 +677,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" hidden="1">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -684,7 +686,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" hidden="1">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -693,7 +695,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" hidden="1">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -702,7 +704,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" hidden="1">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -726,7 +728,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" hidden="1">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -771,7 +773,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" hidden="1">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -795,7 +797,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" hidden="1">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -807,7 +809,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" hidden="1">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -819,7 +821,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" hidden="1">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -828,7 +830,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" hidden="1">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -837,7 +839,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" hidden="1">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -846,7 +848,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" hidden="1">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
@@ -867,7 +869,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" hidden="1">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -876,7 +878,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" hidden="1">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -885,7 +887,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" hidden="1">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
@@ -894,7 +896,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" hidden="1">
       <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
@@ -903,7 +905,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" hidden="1">
       <c r="A31" s="1" t="s">
         <v>17</v>
       </c>
@@ -912,7 +914,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" hidden="1">
       <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
@@ -921,7 +923,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" hidden="1">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -930,7 +932,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" hidden="1">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
@@ -963,7 +965,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" hidden="1">
       <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
@@ -975,7 +977,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" hidden="1">
       <c r="A38" s="1" t="s">
         <v>21</v>
       </c>
@@ -984,7 +986,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" hidden="1">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -993,7 +995,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" hidden="1">
       <c r="A40" s="1" t="s">
         <v>26</v>
       </c>
@@ -1002,7 +1004,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" hidden="1">
       <c r="A41" s="1" t="s">
         <v>27</v>
       </c>
@@ -1011,7 +1013,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" hidden="1">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
@@ -1020,7 +1022,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" hidden="1">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
@@ -1029,7 +1031,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" hidden="1">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
@@ -1038,7 +1040,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" hidden="1">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
@@ -1050,7 +1052,7 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" hidden="1">
       <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
@@ -1059,7 +1061,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" hidden="1">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
@@ -1068,7 +1070,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" hidden="1">
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
@@ -1077,7 +1079,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" hidden="1">
       <c r="A49" s="1" t="s">
         <v>51</v>
       </c>
@@ -1086,7 +1088,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" hidden="1">
       <c r="A50" s="1" t="s">
         <v>52</v>
       </c>
@@ -1095,7 +1097,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" hidden="1">
       <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
@@ -1104,7 +1106,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" hidden="1">
       <c r="A52" s="1" t="s">
         <v>54</v>
       </c>
@@ -1113,7 +1115,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" hidden="1">
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
@@ -1134,7 +1136,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" hidden="1">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" hidden="1">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
@@ -1152,7 +1154,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" hidden="1">
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
@@ -1161,7 +1163,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" hidden="1">
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
@@ -1170,7 +1172,7 @@
         <v>no</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" hidden="1">
       <c r="A59" s="1" t="s">
         <v>61</v>
       </c>
@@ -1180,7 +1182,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{4460966F-A681-4CC4-9BC5-D71793F5778B}"/>
+  <autoFilter ref="A1:C59" xr:uid="{4460966F-A681-4CC4-9BC5-D71793F5778B}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="no"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>